<commit_message>
Retest of UI Automation script for commited modules
</commit_message>
<xml_diff>
--- a/tests/artifact/script/UI-ViewTrialBalance.xlsx
+++ b/tests/artifact/script/UI-ViewTrialBalance.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9252" tabRatio="550" firstSheet="1" activeTab="1"/>
+    <workbookView windowWidth="18350" windowHeight="6950" tabRatio="550" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="857">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1116" uniqueCount="859">
   <si>
     <t>target</t>
   </si>
@@ -2616,6 +2616,12 @@
     <t>${table.rows.trialbalance}[${counter}]${table.accountname.link}</t>
   </si>
   <si>
+    <t>wait for 3 seconds to load the page</t>
+  </si>
+  <si>
+    <t>5000</t>
+  </si>
+  <si>
     <t>validate account name in ledger account page</t>
   </si>
   <si>
@@ -2679,13 +2685,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="5">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="dd\-mm\-yyyy;@"/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="180" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="31">
     <font>
@@ -3265,16 +3271,16 @@
     <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3521,7 +3527,7 @@
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -3997,7 +4003,7 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="18" width="8.33333333333333" customWidth="1" collapsed="1"/>
   </cols>
@@ -6668,13 +6674,13 @@
   <sheetPr/>
   <dimension ref="A1:P225"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="44.5333333333333" style="6" customWidth="1"/>
     <col min="2" max="2" width="42.75" style="7" customWidth="1"/>
@@ -6693,7 +6699,7 @@
     <col min="16" max="16384" width="10.8333333333333" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.15" spans="1:15">
+    <row r="1" ht="15.25" spans="1:15">
       <c r="A1" s="15" t="s">
         <v>725</v>
       </c>
@@ -6724,7 +6730,7 @@
       <c r="N1" s="17"/>
       <c r="O1" s="43"/>
     </row>
-    <row r="2" s="1" customFormat="1" ht="15.15" spans="1:15">
+    <row r="2" s="1" customFormat="1" ht="15.25" spans="1:15">
       <c r="A2" s="18" t="s">
         <v>732</v>
       </c>
@@ -6805,7 +6811,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="5" s="1" customFormat="1" ht="31.2" spans="1:15">
+    <row r="5" s="1" customFormat="1" ht="31" spans="1:15">
       <c r="A5" s="22" t="s">
         <v>746</v>
       </c>
@@ -6834,7 +6840,7 @@
       <c r="N5" s="26"/>
       <c r="O5" s="25"/>
     </row>
-    <row r="6" s="3" customFormat="1" ht="15.6" spans="1:15">
+    <row r="6" s="3" customFormat="1" ht="15.5" spans="1:15">
       <c r="A6" s="22"/>
       <c r="B6" s="63" t="s">
         <v>750</v>
@@ -10739,15 +10745,15 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:P282"/>
+  <dimension ref="A1:P283"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomLeft" activeCell="A48" sqref="A48:D50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="44.5333333333333" style="6" customWidth="1"/>
     <col min="2" max="2" width="42.75" style="7" customWidth="1"/>
@@ -10766,7 +10772,7 @@
     <col min="16" max="16384" width="10.8333333333333" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.15" spans="1:15">
+    <row r="1" ht="15.25" spans="1:15">
       <c r="A1" s="15" t="s">
         <v>725</v>
       </c>
@@ -10797,7 +10803,7 @@
       <c r="N1" s="17"/>
       <c r="O1" s="43"/>
     </row>
-    <row r="2" s="1" customFormat="1" ht="15.15" spans="1:15">
+    <row r="2" s="1" customFormat="1" ht="15.25" spans="1:15">
       <c r="A2" s="18" t="s">
         <v>732</v>
       </c>
@@ -11753,14 +11759,12 @@
         <v>30</v>
       </c>
       <c r="D39" s="40" t="s">
-        <v>530</v>
+        <v>714</v>
       </c>
       <c r="E39" s="29" t="s">
         <v>838</v>
       </c>
-      <c r="F39" s="29" t="s">
-        <v>834</v>
-      </c>
+      <c r="F39" s="29"/>
       <c r="G39" s="29"/>
       <c r="H39" s="29"/>
       <c r="I39" s="29"/>
@@ -11781,10 +11785,14 @@
         <v>30</v>
       </c>
       <c r="D40" s="40" t="s">
-        <v>620</v>
-      </c>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29"/>
+        <v>530</v>
+      </c>
+      <c r="E40" s="29" t="s">
+        <v>840</v>
+      </c>
+      <c r="F40" s="29" t="s">
+        <v>834</v>
+      </c>
       <c r="G40" s="29"/>
       <c r="H40" s="29"/>
       <c r="I40" s="29"/>
@@ -11799,20 +11807,16 @@
     <row r="41" ht="32" customHeight="1" spans="1:16">
       <c r="A41" s="32"/>
       <c r="B41" s="23" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="C41" s="35" t="s">
         <v>30</v>
       </c>
       <c r="D41" s="40" t="s">
-        <v>493</v>
-      </c>
-      <c r="E41" s="31" t="s">
-        <v>841</v>
-      </c>
-      <c r="F41" s="29" t="s">
-        <v>842</v>
-      </c>
+        <v>620</v>
+      </c>
+      <c r="E41" s="29"/>
+      <c r="F41" s="29"/>
       <c r="G41" s="29"/>
       <c r="H41" s="29"/>
       <c r="I41" s="29"/>
@@ -11827,16 +11831,16 @@
     <row r="42" ht="32" customHeight="1" spans="1:16">
       <c r="A42" s="32"/>
       <c r="B42" s="23" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="C42" s="35" t="s">
         <v>30</v>
       </c>
       <c r="D42" s="40" t="s">
-        <v>530</v>
-      </c>
-      <c r="E42" s="29" t="s">
-        <v>842</v>
+        <v>493</v>
+      </c>
+      <c r="E42" s="31" t="s">
+        <v>843</v>
       </c>
       <c r="F42" s="29" t="s">
         <v>844</v>
@@ -11861,13 +11865,13 @@
         <v>30</v>
       </c>
       <c r="D43" s="40" t="s">
-        <v>493</v>
-      </c>
-      <c r="E43" s="31" t="s">
+        <v>530</v>
+      </c>
+      <c r="E43" s="29" t="s">
+        <v>844</v>
+      </c>
+      <c r="F43" s="29" t="s">
         <v>846</v>
-      </c>
-      <c r="F43" s="29" t="s">
-        <v>847</v>
       </c>
       <c r="G43" s="29"/>
       <c r="H43" s="29"/>
@@ -11883,16 +11887,16 @@
     <row r="44" ht="32" customHeight="1" spans="1:16">
       <c r="A44" s="32"/>
       <c r="B44" s="23" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="C44" s="35" t="s">
         <v>30</v>
       </c>
       <c r="D44" s="40" t="s">
-        <v>530</v>
-      </c>
-      <c r="E44" s="29" t="s">
-        <v>847</v>
+        <v>493</v>
+      </c>
+      <c r="E44" s="31" t="s">
+        <v>848</v>
       </c>
       <c r="F44" s="29" t="s">
         <v>849</v>
@@ -11917,13 +11921,13 @@
         <v>30</v>
       </c>
       <c r="D45" s="40" t="s">
-        <v>493</v>
-      </c>
-      <c r="E45" s="31" t="s">
+        <v>530</v>
+      </c>
+      <c r="E45" s="29" t="s">
+        <v>849</v>
+      </c>
+      <c r="F45" s="29" t="s">
         <v>851</v>
-      </c>
-      <c r="F45" s="29" t="s">
-        <v>852</v>
       </c>
       <c r="G45" s="29"/>
       <c r="H45" s="29"/>
@@ -11939,16 +11943,16 @@
     <row r="46" ht="32" customHeight="1" spans="1:16">
       <c r="A46" s="32"/>
       <c r="B46" s="23" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="C46" s="35" t="s">
         <v>30</v>
       </c>
       <c r="D46" s="40" t="s">
-        <v>530</v>
-      </c>
-      <c r="E46" s="29" t="s">
-        <v>852</v>
+        <v>493</v>
+      </c>
+      <c r="E46" s="31" t="s">
+        <v>853</v>
       </c>
       <c r="F46" s="29" t="s">
         <v>854</v>
@@ -11964,24 +11968,22 @@
       <c r="O46" s="29"/>
       <c r="P46" s="29"/>
     </row>
-    <row r="47" ht="34" customHeight="1" spans="1:16">
-      <c r="A47" s="32" t="s">
+    <row r="47" ht="32" customHeight="1" spans="1:16">
+      <c r="A47" s="32"/>
+      <c r="B47" s="23" t="s">
         <v>855</v>
       </c>
-      <c r="B47" s="34" t="s">
-        <v>809</v>
-      </c>
       <c r="C47" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="D47" s="31" t="s">
-        <v>471</v>
-      </c>
-      <c r="E47" s="31" t="s">
-        <v>810</v>
+        <v>30</v>
+      </c>
+      <c r="D47" s="40" t="s">
+        <v>530</v>
+      </c>
+      <c r="E47" s="29" t="s">
+        <v>854</v>
       </c>
       <c r="F47" s="29" t="s">
-        <v>817</v>
+        <v>856</v>
       </c>
       <c r="G47" s="29"/>
       <c r="H47" s="29"/>
@@ -11995,21 +11997,23 @@
       <c r="P47" s="29"/>
     </row>
     <row r="48" ht="34" customHeight="1" spans="1:16">
-      <c r="A48" s="32"/>
-      <c r="B48" s="23" t="s">
-        <v>812</v>
-      </c>
-      <c r="C48" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="D48" s="29" t="s">
-        <v>483</v>
-      </c>
-      <c r="E48" s="29" t="s">
-        <v>813</v>
-      </c>
-      <c r="F48" s="33" t="s">
-        <v>814</v>
+      <c r="A48" s="32" t="s">
+        <v>857</v>
+      </c>
+      <c r="B48" s="34" t="s">
+        <v>809</v>
+      </c>
+      <c r="C48" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" s="31" t="s">
+        <v>471</v>
+      </c>
+      <c r="E48" s="31" t="s">
+        <v>810</v>
+      </c>
+      <c r="F48" s="29" t="s">
+        <v>817</v>
       </c>
       <c r="G48" s="29"/>
       <c r="H48" s="29"/>
@@ -12025,18 +12029,20 @@
     <row r="49" ht="34" customHeight="1" spans="1:16">
       <c r="A49" s="32"/>
       <c r="B49" s="23" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="C49" s="28" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="D49" s="29" t="s">
-        <v>536</v>
+        <v>483</v>
       </c>
       <c r="E49" s="29" t="s">
-        <v>817</v>
-      </c>
-      <c r="F49" s="33"/>
+        <v>813</v>
+      </c>
+      <c r="F49" s="33" t="s">
+        <v>814</v>
+      </c>
       <c r="G49" s="29"/>
       <c r="H49" s="29"/>
       <c r="I49" s="29"/>
@@ -12050,21 +12056,19 @@
     </row>
     <row r="50" ht="34" customHeight="1" spans="1:16">
       <c r="A50" s="32"/>
-      <c r="B50" s="39" t="s">
-        <v>818</v>
-      </c>
-      <c r="C50" s="35" t="s">
+      <c r="B50" s="23" t="s">
+        <v>816</v>
+      </c>
+      <c r="C50" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="D50" s="31" t="s">
-        <v>465</v>
-      </c>
-      <c r="E50" s="31" t="s">
-        <v>856</v>
-      </c>
-      <c r="F50" s="30" t="s">
-        <v>820</v>
-      </c>
+      <c r="D50" s="29" t="s">
+        <v>536</v>
+      </c>
+      <c r="E50" s="29" t="s">
+        <v>817</v>
+      </c>
+      <c r="F50" s="33"/>
       <c r="G50" s="29"/>
       <c r="H50" s="29"/>
       <c r="I50" s="29"/>
@@ -12077,49 +12081,49 @@
       <c r="P50" s="29"/>
     </row>
     <row r="51" ht="34" customHeight="1" spans="1:16">
-      <c r="A51" s="22"/>
-      <c r="B51" s="23" t="s">
-        <v>821</v>
+      <c r="A51" s="32"/>
+      <c r="B51" s="39" t="s">
+        <v>818</v>
       </c>
       <c r="C51" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="D51" s="40" t="s">
-        <v>49</v>
+      <c r="D51" s="31" t="s">
+        <v>465</v>
       </c>
       <c r="E51" s="31" t="s">
-        <v>822</v>
-      </c>
-      <c r="F51" s="29" t="s">
-        <v>817</v>
+        <v>858</v>
+      </c>
+      <c r="F51" s="30" t="s">
+        <v>820</v>
       </c>
       <c r="G51" s="29"/>
-      <c r="H51" s="4"/>
-      <c r="I51" s="4"/>
-      <c r="J51" s="4"/>
-      <c r="K51" s="4"/>
-      <c r="L51" s="4"/>
-      <c r="M51" s="4"/>
-      <c r="N51" s="57"/>
-      <c r="O51" s="57"/>
-      <c r="P51" s="57"/>
+      <c r="H51" s="29"/>
+      <c r="I51" s="29"/>
+      <c r="J51" s="50"/>
+      <c r="K51" s="32"/>
+      <c r="L51" s="23"/>
+      <c r="M51" s="28"/>
+      <c r="N51" s="29"/>
+      <c r="O51" s="29"/>
+      <c r="P51" s="29"/>
     </row>
     <row r="52" ht="34" customHeight="1" spans="1:16">
       <c r="A52" s="22"/>
       <c r="B52" s="23" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C52" s="35" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D52" s="40" t="s">
-        <v>302</v>
+        <v>49</v>
       </c>
       <c r="E52" s="31" t="s">
-        <v>810</v>
-      </c>
-      <c r="F52" s="30" t="s">
-        <v>824</v>
+        <v>822</v>
+      </c>
+      <c r="F52" s="29" t="s">
+        <v>817</v>
       </c>
       <c r="G52" s="29"/>
       <c r="H52" s="4"/>
@@ -12135,19 +12139,19 @@
     <row r="53" ht="34" customHeight="1" spans="1:16">
       <c r="A53" s="22"/>
       <c r="B53" s="23" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="C53" s="35" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D53" s="40" t="s">
-        <v>493</v>
+        <v>302</v>
       </c>
       <c r="E53" s="31" t="s">
-        <v>826</v>
-      </c>
-      <c r="F53" s="29" t="s">
-        <v>827</v>
+        <v>810</v>
+      </c>
+      <c r="F53" s="30" t="s">
+        <v>824</v>
       </c>
       <c r="G53" s="29"/>
       <c r="H53" s="4"/>
@@ -12163,19 +12167,19 @@
     <row r="54" ht="34" customHeight="1" spans="1:16">
       <c r="A54" s="22"/>
       <c r="B54" s="23" t="s">
-        <v>828</v>
+        <v>825</v>
       </c>
       <c r="C54" s="35" t="s">
         <v>30</v>
       </c>
       <c r="D54" s="40" t="s">
-        <v>530</v>
-      </c>
-      <c r="E54" s="29" t="s">
+        <v>493</v>
+      </c>
+      <c r="E54" s="31" t="s">
+        <v>826</v>
+      </c>
+      <c r="F54" s="29" t="s">
         <v>827</v>
-      </c>
-      <c r="F54" s="29" t="s">
-        <v>829</v>
       </c>
       <c r="G54" s="29"/>
       <c r="H54" s="4"/>
@@ -12189,49 +12193,49 @@
       <c r="P54" s="57"/>
     </row>
     <row r="55" ht="34" customHeight="1" spans="1:16">
-      <c r="A55" s="32"/>
+      <c r="A55" s="22"/>
       <c r="B55" s="23" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="C55" s="35" t="s">
         <v>30</v>
       </c>
       <c r="D55" s="40" t="s">
-        <v>493</v>
-      </c>
-      <c r="E55" s="31" t="s">
-        <v>831</v>
+        <v>530</v>
+      </c>
+      <c r="E55" s="29" t="s">
+        <v>827</v>
       </c>
       <c r="F55" s="29" t="s">
-        <v>832</v>
+        <v>829</v>
       </c>
       <c r="G55" s="29"/>
-      <c r="H55" s="29"/>
-      <c r="I55" s="29"/>
-      <c r="J55" s="50"/>
-      <c r="K55" s="42"/>
-      <c r="L55" s="51"/>
-      <c r="M55" s="52"/>
-      <c r="N55" s="58"/>
-      <c r="O55" s="59"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
+      <c r="J55" s="4"/>
+      <c r="K55" s="4"/>
+      <c r="L55" s="4"/>
+      <c r="M55" s="4"/>
+      <c r="N55" s="57"/>
+      <c r="O55" s="57"/>
       <c r="P55" s="57"/>
     </row>
     <row r="56" ht="34" customHeight="1" spans="1:16">
       <c r="A56" s="32"/>
       <c r="B56" s="23" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="C56" s="35" t="s">
         <v>30</v>
       </c>
       <c r="D56" s="40" t="s">
-        <v>530</v>
-      </c>
-      <c r="E56" s="29" t="s">
+        <v>493</v>
+      </c>
+      <c r="E56" s="31" t="s">
+        <v>831</v>
+      </c>
+      <c r="F56" s="29" t="s">
         <v>832</v>
-      </c>
-      <c r="F56" s="29" t="s">
-        <v>834</v>
       </c>
       <c r="G56" s="29"/>
       <c r="H56" s="29"/>
@@ -12245,46 +12249,46 @@
       <c r="P56" s="57"/>
     </row>
     <row r="57" ht="34" customHeight="1" spans="1:16">
-      <c r="A57" s="22"/>
+      <c r="A57" s="32"/>
       <c r="B57" s="23" t="s">
-        <v>840</v>
+        <v>833</v>
       </c>
       <c r="C57" s="35" t="s">
         <v>30</v>
       </c>
       <c r="D57" s="40" t="s">
-        <v>493</v>
-      </c>
-      <c r="E57" s="31" t="s">
-        <v>841</v>
+        <v>530</v>
+      </c>
+      <c r="E57" s="29" t="s">
+        <v>832</v>
       </c>
       <c r="F57" s="29" t="s">
-        <v>842</v>
+        <v>834</v>
       </c>
       <c r="G57" s="29"/>
-      <c r="H57" s="31"/>
-      <c r="I57" s="31"/>
-      <c r="J57" s="30"/>
-      <c r="K57" s="25"/>
-      <c r="L57" s="26"/>
-      <c r="M57" s="24"/>
-      <c r="N57" s="55"/>
-      <c r="O57" s="54"/>
-      <c r="P57" s="5"/>
+      <c r="H57" s="29"/>
+      <c r="I57" s="29"/>
+      <c r="J57" s="50"/>
+      <c r="K57" s="42"/>
+      <c r="L57" s="51"/>
+      <c r="M57" s="52"/>
+      <c r="N57" s="58"/>
+      <c r="O57" s="59"/>
+      <c r="P57" s="57"/>
     </row>
     <row r="58" ht="34" customHeight="1" spans="1:16">
       <c r="A58" s="22"/>
       <c r="B58" s="23" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="C58" s="35" t="s">
         <v>30</v>
       </c>
       <c r="D58" s="40" t="s">
-        <v>530</v>
-      </c>
-      <c r="E58" s="29" t="s">
-        <v>842</v>
+        <v>493</v>
+      </c>
+      <c r="E58" s="31" t="s">
+        <v>843</v>
       </c>
       <c r="F58" s="29" t="s">
         <v>844</v>
@@ -12301,7 +12305,7 @@
       <c r="P58" s="5"/>
     </row>
     <row r="59" ht="34" customHeight="1" spans="1:16">
-      <c r="A59" s="32"/>
+      <c r="A59" s="22"/>
       <c r="B59" s="23" t="s">
         <v>845</v>
       </c>
@@ -12309,38 +12313,38 @@
         <v>30</v>
       </c>
       <c r="D59" s="40" t="s">
-        <v>493</v>
-      </c>
-      <c r="E59" s="31" t="s">
+        <v>530</v>
+      </c>
+      <c r="E59" s="29" t="s">
+        <v>844</v>
+      </c>
+      <c r="F59" s="29" t="s">
         <v>846</v>
       </c>
-      <c r="F59" s="29" t="s">
-        <v>847</v>
-      </c>
       <c r="G59" s="29"/>
-      <c r="H59" s="29"/>
-      <c r="I59" s="29"/>
-      <c r="J59" s="50"/>
-      <c r="K59" s="42"/>
-      <c r="L59" s="51"/>
-      <c r="M59" s="52"/>
-      <c r="N59" s="58"/>
-      <c r="O59" s="59"/>
-      <c r="P59" s="60"/>
+      <c r="H59" s="31"/>
+      <c r="I59" s="31"/>
+      <c r="J59" s="30"/>
+      <c r="K59" s="25"/>
+      <c r="L59" s="26"/>
+      <c r="M59" s="24"/>
+      <c r="N59" s="55"/>
+      <c r="O59" s="54"/>
+      <c r="P59" s="5"/>
     </row>
     <row r="60" ht="34" customHeight="1" spans="1:16">
       <c r="A60" s="32"/>
       <c r="B60" s="23" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="C60" s="35" t="s">
         <v>30</v>
       </c>
       <c r="D60" s="40" t="s">
-        <v>530</v>
-      </c>
-      <c r="E60" s="29" t="s">
-        <v>847</v>
+        <v>493</v>
+      </c>
+      <c r="E60" s="31" t="s">
+        <v>848</v>
       </c>
       <c r="F60" s="29" t="s">
         <v>849</v>
@@ -12365,13 +12369,13 @@
         <v>30</v>
       </c>
       <c r="D61" s="40" t="s">
-        <v>493</v>
-      </c>
-      <c r="E61" s="31" t="s">
+        <v>530</v>
+      </c>
+      <c r="E61" s="29" t="s">
+        <v>849</v>
+      </c>
+      <c r="F61" s="29" t="s">
         <v>851</v>
-      </c>
-      <c r="F61" s="29" t="s">
-        <v>852</v>
       </c>
       <c r="G61" s="29"/>
       <c r="H61" s="29"/>
@@ -12387,16 +12391,16 @@
     <row r="62" ht="34" customHeight="1" spans="1:16">
       <c r="A62" s="32"/>
       <c r="B62" s="23" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="C62" s="35" t="s">
         <v>30</v>
       </c>
       <c r="D62" s="40" t="s">
-        <v>530</v>
-      </c>
-      <c r="E62" s="29" t="s">
-        <v>852</v>
+        <v>493</v>
+      </c>
+      <c r="E62" s="31" t="s">
+        <v>853</v>
       </c>
       <c r="F62" s="29" t="s">
         <v>854</v>
@@ -12414,11 +12418,21 @@
     </row>
     <row r="63" ht="34" customHeight="1" spans="1:16">
       <c r="A63" s="32"/>
-      <c r="B63" s="39"/>
-      <c r="C63" s="35"/>
-      <c r="D63" s="31"/>
-      <c r="E63" s="31"/>
-      <c r="F63" s="31"/>
+      <c r="B63" s="23" t="s">
+        <v>855</v>
+      </c>
+      <c r="C63" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D63" s="40" t="s">
+        <v>530</v>
+      </c>
+      <c r="E63" s="29" t="s">
+        <v>854</v>
+      </c>
+      <c r="F63" s="29" t="s">
+        <v>856</v>
+      </c>
       <c r="G63" s="29"/>
       <c r="H63" s="29"/>
       <c r="I63" s="29"/>
@@ -12433,10 +12447,10 @@
     <row r="64" ht="34" customHeight="1" spans="1:16">
       <c r="A64" s="32"/>
       <c r="B64" s="39"/>
-      <c r="C64" s="28"/>
-      <c r="D64" s="29"/>
-      <c r="E64" s="29"/>
-      <c r="F64" s="29"/>
+      <c r="C64" s="35"/>
+      <c r="D64" s="31"/>
+      <c r="E64" s="31"/>
+      <c r="F64" s="31"/>
       <c r="G64" s="29"/>
       <c r="H64" s="29"/>
       <c r="I64" s="29"/>
@@ -12451,10 +12465,10 @@
     <row r="65" ht="34" customHeight="1" spans="1:16">
       <c r="A65" s="32"/>
       <c r="B65" s="39"/>
-      <c r="C65" s="35"/>
-      <c r="D65" s="31"/>
-      <c r="E65" s="31"/>
-      <c r="F65" s="31"/>
+      <c r="C65" s="28"/>
+      <c r="D65" s="29"/>
+      <c r="E65" s="29"/>
+      <c r="F65" s="29"/>
       <c r="G65" s="29"/>
       <c r="H65" s="29"/>
       <c r="I65" s="29"/>
@@ -12469,10 +12483,10 @@
     <row r="66" ht="34" customHeight="1" spans="1:16">
       <c r="A66" s="32"/>
       <c r="B66" s="39"/>
-      <c r="C66" s="28"/>
-      <c r="D66" s="29"/>
-      <c r="E66" s="29"/>
-      <c r="F66" s="29"/>
+      <c r="C66" s="35"/>
+      <c r="D66" s="31"/>
+      <c r="E66" s="31"/>
+      <c r="F66" s="31"/>
       <c r="G66" s="29"/>
       <c r="H66" s="29"/>
       <c r="I66" s="29"/>
@@ -12487,10 +12501,10 @@
     <row r="67" ht="34" customHeight="1" spans="1:16">
       <c r="A67" s="32"/>
       <c r="B67" s="39"/>
-      <c r="C67" s="35"/>
-      <c r="D67" s="31"/>
-      <c r="E67" s="31"/>
-      <c r="F67" s="31"/>
+      <c r="C67" s="28"/>
+      <c r="D67" s="29"/>
+      <c r="E67" s="29"/>
+      <c r="F67" s="29"/>
       <c r="G67" s="29"/>
       <c r="H67" s="29"/>
       <c r="I67" s="29"/>
@@ -12505,10 +12519,10 @@
     <row r="68" ht="34" customHeight="1" spans="1:16">
       <c r="A68" s="32"/>
       <c r="B68" s="39"/>
-      <c r="C68" s="28"/>
-      <c r="D68" s="29"/>
-      <c r="E68" s="29"/>
-      <c r="F68" s="29"/>
+      <c r="C68" s="35"/>
+      <c r="D68" s="31"/>
+      <c r="E68" s="31"/>
+      <c r="F68" s="31"/>
       <c r="G68" s="29"/>
       <c r="H68" s="29"/>
       <c r="I68" s="29"/>
@@ -12523,10 +12537,10 @@
     <row r="69" ht="34" customHeight="1" spans="1:16">
       <c r="A69" s="32"/>
       <c r="B69" s="39"/>
-      <c r="C69" s="35"/>
-      <c r="D69" s="31"/>
-      <c r="E69" s="31"/>
-      <c r="F69" s="31"/>
+      <c r="C69" s="28"/>
+      <c r="D69" s="29"/>
+      <c r="E69" s="29"/>
+      <c r="F69" s="29"/>
       <c r="G69" s="29"/>
       <c r="H69" s="29"/>
       <c r="I69" s="29"/>
@@ -12543,7 +12557,7 @@
       <c r="B70" s="39"/>
       <c r="C70" s="35"/>
       <c r="D70" s="31"/>
-      <c r="E70" s="29"/>
+      <c r="E70" s="31"/>
       <c r="F70" s="31"/>
       <c r="G70" s="29"/>
       <c r="H70" s="29"/>
@@ -12559,10 +12573,10 @@
     <row r="71" ht="34" customHeight="1" spans="1:16">
       <c r="A71" s="32"/>
       <c r="B71" s="39"/>
-      <c r="C71" s="28"/>
-      <c r="D71" s="29"/>
+      <c r="C71" s="35"/>
+      <c r="D71" s="31"/>
       <c r="E71" s="29"/>
-      <c r="F71" s="29"/>
+      <c r="F71" s="31"/>
       <c r="G71" s="29"/>
       <c r="H71" s="29"/>
       <c r="I71" s="29"/>
@@ -12613,10 +12627,10 @@
     <row r="74" ht="34" customHeight="1" spans="1:16">
       <c r="A74" s="32"/>
       <c r="B74" s="39"/>
-      <c r="C74" s="35"/>
-      <c r="D74" s="31"/>
-      <c r="E74" s="31"/>
-      <c r="F74" s="31"/>
+      <c r="C74" s="28"/>
+      <c r="D74" s="29"/>
+      <c r="E74" s="29"/>
+      <c r="F74" s="29"/>
       <c r="G74" s="29"/>
       <c r="H74" s="29"/>
       <c r="I74" s="29"/>
@@ -12631,10 +12645,10 @@
     <row r="75" ht="34" customHeight="1" spans="1:16">
       <c r="A75" s="32"/>
       <c r="B75" s="39"/>
-      <c r="C75" s="28"/>
-      <c r="D75" s="29"/>
-      <c r="E75" s="29"/>
-      <c r="F75" s="14"/>
+      <c r="C75" s="35"/>
+      <c r="D75" s="31"/>
+      <c r="E75" s="31"/>
+      <c r="F75" s="31"/>
       <c r="G75" s="29"/>
       <c r="H75" s="29"/>
       <c r="I75" s="29"/>
@@ -12652,7 +12666,7 @@
       <c r="C76" s="28"/>
       <c r="D76" s="29"/>
       <c r="E76" s="29"/>
-      <c r="F76" s="29"/>
+      <c r="F76" s="14"/>
       <c r="G76" s="29"/>
       <c r="H76" s="29"/>
       <c r="I76" s="29"/>
@@ -12670,7 +12684,7 @@
       <c r="C77" s="28"/>
       <c r="D77" s="29"/>
       <c r="E77" s="29"/>
-      <c r="F77" s="14"/>
+      <c r="F77" s="29"/>
       <c r="G77" s="29"/>
       <c r="H77" s="29"/>
       <c r="I77" s="29"/>
@@ -12685,10 +12699,10 @@
     <row r="78" ht="34" customHeight="1" spans="1:16">
       <c r="A78" s="32"/>
       <c r="B78" s="39"/>
-      <c r="C78" s="35"/>
-      <c r="D78" s="31"/>
-      <c r="E78" s="31"/>
-      <c r="F78" s="31"/>
+      <c r="C78" s="28"/>
+      <c r="D78" s="29"/>
+      <c r="E78" s="29"/>
+      <c r="F78" s="14"/>
       <c r="G78" s="29"/>
       <c r="H78" s="29"/>
       <c r="I78" s="29"/>
@@ -12703,9 +12717,9 @@
     <row r="79" ht="34" customHeight="1" spans="1:16">
       <c r="A79" s="32"/>
       <c r="B79" s="39"/>
-      <c r="C79" s="28"/>
-      <c r="D79" s="29"/>
-      <c r="E79" s="29"/>
+      <c r="C79" s="35"/>
+      <c r="D79" s="31"/>
+      <c r="E79" s="31"/>
       <c r="F79" s="31"/>
       <c r="G79" s="29"/>
       <c r="H79" s="29"/>
@@ -12760,7 +12774,7 @@
       <c r="C82" s="28"/>
       <c r="D82" s="29"/>
       <c r="E82" s="29"/>
-      <c r="F82" s="29"/>
+      <c r="F82" s="31"/>
       <c r="G82" s="29"/>
       <c r="H82" s="29"/>
       <c r="I82" s="29"/>
@@ -12775,10 +12789,10 @@
     <row r="83" ht="34" customHeight="1" spans="1:16">
       <c r="A83" s="32"/>
       <c r="B83" s="39"/>
-      <c r="C83" s="35"/>
-      <c r="D83" s="31"/>
-      <c r="E83" s="31"/>
-      <c r="F83" s="31"/>
+      <c r="C83" s="28"/>
+      <c r="D83" s="29"/>
+      <c r="E83" s="29"/>
+      <c r="F83" s="29"/>
       <c r="G83" s="29"/>
       <c r="H83" s="29"/>
       <c r="I83" s="29"/>
@@ -12793,10 +12807,10 @@
     <row r="84" ht="34" customHeight="1" spans="1:16">
       <c r="A84" s="32"/>
       <c r="B84" s="39"/>
-      <c r="C84" s="28"/>
-      <c r="D84" s="29"/>
-      <c r="E84" s="29"/>
-      <c r="F84" s="29"/>
+      <c r="C84" s="35"/>
+      <c r="D84" s="31"/>
+      <c r="E84" s="31"/>
+      <c r="F84" s="31"/>
       <c r="G84" s="29"/>
       <c r="H84" s="29"/>
       <c r="I84" s="29"/>
@@ -12811,10 +12825,10 @@
     <row r="85" ht="34" customHeight="1" spans="1:16">
       <c r="A85" s="32"/>
       <c r="B85" s="39"/>
-      <c r="C85" s="35"/>
-      <c r="D85" s="31"/>
-      <c r="E85" s="31"/>
-      <c r="F85" s="31"/>
+      <c r="C85" s="28"/>
+      <c r="D85" s="29"/>
+      <c r="E85" s="29"/>
+      <c r="F85" s="29"/>
       <c r="G85" s="29"/>
       <c r="H85" s="29"/>
       <c r="I85" s="29"/>
@@ -12829,10 +12843,10 @@
     <row r="86" ht="34" customHeight="1" spans="1:16">
       <c r="A86" s="32"/>
       <c r="B86" s="39"/>
-      <c r="C86" s="28"/>
-      <c r="D86" s="29"/>
-      <c r="E86" s="29"/>
-      <c r="F86" s="29"/>
+      <c r="C86" s="35"/>
+      <c r="D86" s="31"/>
+      <c r="E86" s="31"/>
+      <c r="F86" s="31"/>
       <c r="G86" s="29"/>
       <c r="H86" s="29"/>
       <c r="I86" s="29"/>
@@ -12847,10 +12861,10 @@
     <row r="87" ht="34" customHeight="1" spans="1:16">
       <c r="A87" s="32"/>
       <c r="B87" s="39"/>
-      <c r="C87" s="35"/>
-      <c r="D87" s="31"/>
-      <c r="E87" s="31"/>
-      <c r="F87" s="31"/>
+      <c r="C87" s="28"/>
+      <c r="D87" s="29"/>
+      <c r="E87" s="29"/>
+      <c r="F87" s="29"/>
       <c r="G87" s="29"/>
       <c r="H87" s="29"/>
       <c r="I87" s="29"/>
@@ -12867,7 +12881,7 @@
       <c r="B88" s="39"/>
       <c r="C88" s="35"/>
       <c r="D88" s="31"/>
-      <c r="E88" s="29"/>
+      <c r="E88" s="31"/>
       <c r="F88" s="31"/>
       <c r="G88" s="29"/>
       <c r="H88" s="29"/>
@@ -12883,10 +12897,10 @@
     <row r="89" ht="34" customHeight="1" spans="1:16">
       <c r="A89" s="32"/>
       <c r="B89" s="39"/>
-      <c r="C89" s="28"/>
-      <c r="D89" s="29"/>
+      <c r="C89" s="35"/>
+      <c r="D89" s="31"/>
       <c r="E89" s="29"/>
-      <c r="F89" s="29"/>
+      <c r="F89" s="31"/>
       <c r="G89" s="29"/>
       <c r="H89" s="29"/>
       <c r="I89" s="29"/>
@@ -13120,7 +13134,7 @@
       <c r="C102" s="28"/>
       <c r="D102" s="29"/>
       <c r="E102" s="29"/>
-      <c r="F102" s="31"/>
+      <c r="F102" s="29"/>
       <c r="G102" s="29"/>
       <c r="H102" s="29"/>
       <c r="I102" s="29"/>
@@ -13174,7 +13188,7 @@
       <c r="C105" s="28"/>
       <c r="D105" s="29"/>
       <c r="E105" s="29"/>
-      <c r="F105" s="29"/>
+      <c r="F105" s="31"/>
       <c r="G105" s="29"/>
       <c r="H105" s="29"/>
       <c r="I105" s="29"/>
@@ -13189,10 +13203,10 @@
     <row r="106" ht="34" customHeight="1" spans="1:16">
       <c r="A106" s="32"/>
       <c r="B106" s="39"/>
-      <c r="C106" s="35"/>
-      <c r="D106" s="31"/>
-      <c r="E106" s="31"/>
-      <c r="F106" s="31"/>
+      <c r="C106" s="28"/>
+      <c r="D106" s="29"/>
+      <c r="E106" s="29"/>
+      <c r="F106" s="29"/>
       <c r="G106" s="29"/>
       <c r="H106" s="29"/>
       <c r="I106" s="29"/>
@@ -13209,7 +13223,7 @@
       <c r="B107" s="39"/>
       <c r="C107" s="35"/>
       <c r="D107" s="31"/>
-      <c r="E107" s="29"/>
+      <c r="E107" s="31"/>
       <c r="F107" s="31"/>
       <c r="G107" s="29"/>
       <c r="H107" s="29"/>
@@ -13225,10 +13239,10 @@
     <row r="108" ht="34" customHeight="1" spans="1:16">
       <c r="A108" s="32"/>
       <c r="B108" s="39"/>
-      <c r="C108" s="28"/>
-      <c r="D108" s="29"/>
+      <c r="C108" s="35"/>
+      <c r="D108" s="31"/>
       <c r="E108" s="29"/>
-      <c r="F108" s="29"/>
+      <c r="F108" s="31"/>
       <c r="G108" s="29"/>
       <c r="H108" s="29"/>
       <c r="I108" s="29"/>
@@ -13240,7 +13254,7 @@
       <c r="O108" s="59"/>
       <c r="P108" s="60"/>
     </row>
-    <row r="109" ht="34" customHeight="1" spans="1:15">
+    <row r="109" ht="34" customHeight="1" spans="1:16">
       <c r="A109" s="32"/>
       <c r="B109" s="39"/>
       <c r="C109" s="28"/>
@@ -13254,8 +13268,9 @@
       <c r="K109" s="42"/>
       <c r="L109" s="51"/>
       <c r="M109" s="52"/>
-      <c r="N109" s="51"/>
-      <c r="O109" s="42"/>
+      <c r="N109" s="58"/>
+      <c r="O109" s="59"/>
+      <c r="P109" s="60"/>
     </row>
     <row r="110" ht="34" customHeight="1" spans="1:15">
       <c r="A110" s="32"/>
@@ -13331,7 +13346,7 @@
       <c r="C114" s="28"/>
       <c r="D114" s="29"/>
       <c r="E114" s="29"/>
-      <c r="F114" s="31"/>
+      <c r="F114" s="29"/>
       <c r="G114" s="29"/>
       <c r="H114" s="29"/>
       <c r="I114" s="29"/>
@@ -13382,7 +13397,7 @@
       <c r="C117" s="28"/>
       <c r="D117" s="29"/>
       <c r="E117" s="29"/>
-      <c r="F117" s="29"/>
+      <c r="F117" s="31"/>
       <c r="G117" s="29"/>
       <c r="H117" s="29"/>
       <c r="I117" s="29"/>
@@ -13396,10 +13411,10 @@
     <row r="118" ht="34" customHeight="1" spans="1:15">
       <c r="A118" s="32"/>
       <c r="B118" s="39"/>
-      <c r="C118" s="35"/>
-      <c r="D118" s="31"/>
-      <c r="E118" s="31"/>
-      <c r="F118" s="31"/>
+      <c r="C118" s="28"/>
+      <c r="D118" s="29"/>
+      <c r="E118" s="29"/>
+      <c r="F118" s="29"/>
       <c r="G118" s="29"/>
       <c r="H118" s="29"/>
       <c r="I118" s="29"/>
@@ -13410,31 +13425,30 @@
       <c r="N118" s="51"/>
       <c r="O118" s="42"/>
     </row>
-    <row r="119" ht="23" customHeight="1" spans="1:16">
-      <c r="A119" s="22"/>
-      <c r="B119" s="23"/>
-      <c r="C119" s="28"/>
-      <c r="D119" s="29"/>
-      <c r="E119" s="61"/>
-      <c r="F119" s="29"/>
+    <row r="119" ht="34" customHeight="1" spans="1:15">
+      <c r="A119" s="32"/>
+      <c r="B119" s="39"/>
+      <c r="C119" s="35"/>
+      <c r="D119" s="31"/>
+      <c r="E119" s="31"/>
+      <c r="F119" s="31"/>
       <c r="G119" s="29"/>
       <c r="H119" s="29"/>
       <c r="I119" s="29"/>
       <c r="J119" s="50"/>
-      <c r="K119" s="32"/>
-      <c r="L119" s="23"/>
-      <c r="M119" s="28"/>
-      <c r="N119" s="29"/>
-      <c r="O119" s="29"/>
-      <c r="P119" s="29"/>
-    </row>
-    <row r="120" s="1" customFormat="1" ht="23" customHeight="1" spans="1:16">
-      <c r="A120" s="32"/>
+      <c r="K119" s="42"/>
+      <c r="L119" s="51"/>
+      <c r="M119" s="52"/>
+      <c r="N119" s="51"/>
+      <c r="O119" s="42"/>
+    </row>
+    <row r="120" ht="23" customHeight="1" spans="1:16">
+      <c r="A120" s="22"/>
       <c r="B120" s="23"/>
       <c r="C120" s="28"/>
       <c r="D120" s="29"/>
       <c r="E120" s="61"/>
-      <c r="F120" s="33"/>
+      <c r="F120" s="29"/>
       <c r="G120" s="29"/>
       <c r="H120" s="29"/>
       <c r="I120" s="29"/>
@@ -13446,12 +13460,12 @@
       <c r="O120" s="29"/>
       <c r="P120" s="29"/>
     </row>
-    <row r="121" s="5" customFormat="1" ht="23" customHeight="1" spans="1:16">
+    <row r="121" s="1" customFormat="1" ht="23" customHeight="1" spans="1:16">
       <c r="A121" s="32"/>
       <c r="B121" s="23"/>
       <c r="C121" s="28"/>
       <c r="D121" s="29"/>
-      <c r="E121" s="29"/>
+      <c r="E121" s="61"/>
       <c r="F121" s="33"/>
       <c r="G121" s="29"/>
       <c r="H121" s="29"/>
@@ -13482,7 +13496,7 @@
       <c r="O122" s="29"/>
       <c r="P122" s="29"/>
     </row>
-    <row r="123" ht="23" customHeight="1" spans="1:16">
+    <row r="123" s="5" customFormat="1" ht="23" customHeight="1" spans="1:16">
       <c r="A123" s="32"/>
       <c r="B123" s="23"/>
       <c r="C123" s="28"/>
@@ -13506,7 +13520,7 @@
       <c r="C124" s="28"/>
       <c r="D124" s="29"/>
       <c r="E124" s="29"/>
-      <c r="F124" s="29"/>
+      <c r="F124" s="33"/>
       <c r="G124" s="29"/>
       <c r="H124" s="29"/>
       <c r="I124" s="29"/>
@@ -16020,9 +16034,9 @@
       <c r="O263" s="29"/>
       <c r="P263" s="29"/>
     </row>
-    <row r="264" ht="23" customHeight="1" spans="1:15">
+    <row r="264" ht="23" customHeight="1" spans="1:16">
       <c r="A264" s="32"/>
-      <c r="B264" s="39"/>
+      <c r="B264" s="23"/>
       <c r="C264" s="28"/>
       <c r="D264" s="29"/>
       <c r="E264" s="29"/>
@@ -16031,11 +16045,12 @@
       <c r="H264" s="29"/>
       <c r="I264" s="29"/>
       <c r="J264" s="50"/>
-      <c r="K264" s="42"/>
-      <c r="L264" s="51"/>
-      <c r="M264" s="52"/>
-      <c r="N264" s="51"/>
-      <c r="O264" s="42"/>
+      <c r="K264" s="32"/>
+      <c r="L264" s="23"/>
+      <c r="M264" s="28"/>
+      <c r="N264" s="29"/>
+      <c r="O264" s="29"/>
+      <c r="P264" s="29"/>
     </row>
     <row r="265" ht="23" customHeight="1" spans="1:15">
       <c r="A265" s="32"/>
@@ -16342,6 +16357,23 @@
       <c r="M282" s="52"/>
       <c r="N282" s="51"/>
       <c r="O282" s="42"/>
+    </row>
+    <row r="283" ht="23" customHeight="1" spans="1:15">
+      <c r="A283" s="32"/>
+      <c r="B283" s="39"/>
+      <c r="C283" s="28"/>
+      <c r="D283" s="29"/>
+      <c r="E283" s="29"/>
+      <c r="F283" s="29"/>
+      <c r="G283" s="29"/>
+      <c r="H283" s="29"/>
+      <c r="I283" s="29"/>
+      <c r="J283" s="50"/>
+      <c r="K283" s="42"/>
+      <c r="L283" s="51"/>
+      <c r="M283" s="52"/>
+      <c r="N283" s="51"/>
+      <c r="O283" s="42"/>
     </row>
   </sheetData>
   <sheetProtection insertRows="0" insertHyperlinks="0" deleteRows="0"/>
@@ -16417,88 +16449,88 @@
       <formula>LEFT(N21,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N55:N56">
+  <conditionalFormatting sqref="N56:N57">
     <cfRule type="beginsWith" dxfId="2" priority="10" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N55,LEN("WARN"))="WARN"</formula>
+      <formula>LEFT(N56,LEN("WARN"))="WARN"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="11" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N55,LEN("FAIL"))="FAIL"</formula>
+      <formula>LEFT(N56,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="0" priority="12" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N55,LEN("PASS"))="PASS"</formula>
+      <formula>LEFT(N56,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N57:N58">
+  <conditionalFormatting sqref="N58:N59">
     <cfRule type="beginsWith" dxfId="2" priority="7" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N57,LEN("WARN"))="WARN"</formula>
+      <formula>LEFT(N58,LEN("WARN"))="WARN"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="8" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N57,LEN("FAIL"))="FAIL"</formula>
+      <formula>LEFT(N58,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="0" priority="9" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N57,LEN("PASS"))="PASS"</formula>
+      <formula>LEFT(N58,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N59:N60">
+  <conditionalFormatting sqref="N60:N61">
     <cfRule type="beginsWith" dxfId="2" priority="19" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N59,LEN("WARN"))="WARN"</formula>
+      <formula>LEFT(N60,LEN("WARN"))="WARN"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="20" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N59,LEN("FAIL"))="FAIL"</formula>
+      <formula>LEFT(N60,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="0" priority="21" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N59,LEN("PASS"))="PASS"</formula>
+      <formula>LEFT(N60,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N66:N67">
+  <conditionalFormatting sqref="N67:N68">
     <cfRule type="beginsWith" dxfId="2" priority="4" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N66,LEN("WARN"))="WARN"</formula>
+      <formula>LEFT(N67,LEN("WARN"))="WARN"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="5" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N66,LEN("FAIL"))="FAIL"</formula>
+      <formula>LEFT(N67,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="0" priority="6" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N66,LEN("PASS"))="PASS"</formula>
+      <formula>LEFT(N67,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N68:N69">
+  <conditionalFormatting sqref="N69:N70">
     <cfRule type="beginsWith" dxfId="2" priority="1" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N68,LEN("WARN"))="WARN"</formula>
+      <formula>LEFT(N69,LEN("WARN"))="WARN"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="2" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N68,LEN("FAIL"))="FAIL"</formula>
+      <formula>LEFT(N69,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="0" priority="3" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N68,LEN("PASS"))="PASS"</formula>
+      <formula>LEFT(N69,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N264:N282">
+  <conditionalFormatting sqref="N265:N283">
     <cfRule type="beginsWith" dxfId="2" priority="40" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N264,LEN("WARN"))="WARN"</formula>
+      <formula>LEFT(N265,LEN("WARN"))="WARN"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="41" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N264,LEN("FAIL"))="FAIL"</formula>
+      <formula>LEFT(N265,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="0" priority="42" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N264,LEN("PASS"))="PASS"</formula>
+      <formula>LEFT(N265,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N61:N65 N70:N118">
+  <conditionalFormatting sqref="N62:N66 N71:N119">
     <cfRule type="beginsWith" dxfId="2" priority="16" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N61,LEN("WARN"))="WARN"</formula>
+      <formula>LEFT(N62,LEN("WARN"))="WARN"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="17" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N61,LEN("FAIL"))="FAIL"</formula>
+      <formula>LEFT(N62,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="0" priority="18" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N61,LEN("PASS"))="PASS"</formula>
+      <formula>LEFT(N62,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 C6 C7 C8 C9 C10 C11 C12 C13 C14 C15 C16 C17 C18 C19 C20 C21 C22 C23 C24 C25 C26 C27 C28 C29 C30 C33 C47 C48 C49 C52 C63 C64 C65 C66 C67 C68 C69 C70 C71 C72 C73 C74 C75 C76 C77 C78 C79 C82 C83 C84 C85 C86 C87 C88 C89 C90 C91 C92 C93 C94 C97 C100 C101 C102 C105 C106 C107 C108 C111 C112 C113 C114 C117 C118 C119 C120 C31:C32 C34:C35 C36:C37 C38:C40 C41:C42 C43:C44 C45:C46 C50:C51 C53:C54 C55:C56 C57:C58 C59:C60 C61:C62 C80:C81 C95:C96 C98:C99 C103:C104 C109:C110 C115:C116 C121:C123 C124:C177 C178:C219 C220:C282">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 C6 C7 C8 C9 C10 C11 C12 C13 C14 C15 C16 C17 C18 C19 C20 C21 C22 C23 C24 C25 C26 C27 C28 C29 C30 C33 C38 C39 C48 C49 C50 C53 C64 C65 C66 C67 C68 C69 C70 C71 C72 C73 C74 C75 C76 C77 C78 C79 C80 C83 C84 C85 C86 C87 C88 C89 C90 C91 C92 C93 C94 C95 C98 C101 C102 C103 C106 C107 C108 C109 C112 C113 C114 C115 C118 C119 C120 C121 C31:C32 C34:C35 C36:C37 C40:C41 C42:C43 C44:C45 C46:C47 C51:C52 C54:C55 C56:C57 C58:C59 C60:C61 C62:C63 C81:C82 C96:C97 C99:C100 C104:C105 C110:C111 C116:C117 C122:C124 C125:C178 C179:C220 C221:C283">
       <formula1>target</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5 D6 D7 D8 D9 D10 D11 D12 D13 D14 D15 D16 D17 D18 D19 D20 D21 D22 D23 D24 D25 D26 D27 D28 D29 D30 D33 D47 D48 D49 D52 D63 D64 D65 D66 D67 D68 D69 D70 D71 D72 D73 D74 D75 D76 D77 D78 D79 D82 D83 D84 D85 D86 D87 D88 D89 D90 D91 D92 D93 D94 D97 D98 D99 D100 D101 D102 D105 D106 D107 D108 D111 D112 D113 D114 D117 D118 D119 D120 D31:D32 D34:D35 D36:D37 D38:D40 D41:D42 D43:D44 D45:D46 D50:D51 D53:D54 D55:D56 D57:D58 D59:D60 D61:D62 D80:D81 D95:D96 D103:D104 D109:D110 D115:D116 D121:D123 D124:D166 D167:D282">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5 D6 D7 D8 D9 D10 D11 D12 D13 D14 D15 D16 D17 D18 D19 D20 D21 D22 D23 D24 D25 D26 D27 D28 D29 D30 D33 D38 D39 D48 D49 D50 D53 D64 D65 D66 D67 D68 D69 D70 D71 D72 D73 D74 D75 D76 D77 D78 D79 D80 D83 D84 D85 D86 D87 D88 D89 D90 D91 D92 D93 D94 D95 D98 D99 D100 D101 D102 D103 D106 D107 D108 D109 D112 D113 D114 D115 D118 D119 D120 D121 D31:D32 D34:D35 D36:D37 D40:D41 D42:D43 D44:D45 D46:D47 D51:D52 D54:D55 D56:D57 D58:D59 D60:D61 D62:D63 D81:D82 D96:D97 D104:D105 D110:D111 D116:D117 D122:D124 D125:D167 D168:D283">
       <formula1>INDIRECT(C5)</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>